<commit_message>
final updates for 2018
</commit_message>
<xml_diff>
--- a/Lectures/lecture8_data/BreastCancer_Clinical.xlsx
+++ b/Lectures/lecture8_data/BreastCancer_Clinical.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhijit/ARAASTAT/FAES/BIOF339_PracticalR/Lectures/lecture8_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C35070-5C3E-4E4E-9C96-D887512FA22B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-19660" yWindow="1260" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cllinical" sheetId="1" r:id="rId1"/>
+    <sheet name="Expression" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="193">
   <si>
     <t>Gender</t>
   </si>
@@ -551,13 +558,55 @@
   </si>
   <si>
     <t>ReacI</t>
+  </si>
+  <si>
+    <t>TCGA_ID</t>
+  </si>
+  <si>
+    <t>NP_958782</t>
+  </si>
+  <si>
+    <t>NP_958785</t>
+  </si>
+  <si>
+    <t>NP_958786</t>
+  </si>
+  <si>
+    <t>NP_000436</t>
+  </si>
+  <si>
+    <t>NP_958781</t>
+  </si>
+  <si>
+    <t>NP_958780</t>
+  </si>
+  <si>
+    <t>NP_958783</t>
+  </si>
+  <si>
+    <t>NP_958784</t>
+  </si>
+  <si>
+    <t>NP_112598</t>
+  </si>
+  <si>
+    <t>NP_001611</t>
+  </si>
+  <si>
+    <t>263d3f-I.CPTAC</t>
+  </si>
+  <si>
+    <t>blcdb9-I.CPTAC</t>
+  </si>
+  <si>
+    <t>c4155b-C.CPTAC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,6 +669,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -666,7 +723,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -698,9 +755,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -732,6 +807,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -907,14 +1000,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1006,7 +1099,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1098,7 +1191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1190,7 +1283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1282,7 +1375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1374,7 +1467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1463,7 +1556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1552,7 +1645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1641,7 +1734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1730,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -1819,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -1908,7 +2001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -1997,7 +2090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -2086,7 +2179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -2175,7 +2268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -2264,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2353,7 +2446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -2442,7 +2535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
@@ -2531,7 +2624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -2620,7 +2713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -2709,7 +2802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
@@ -2798,7 +2891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -2887,7 +2980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
@@ -2976,7 +3069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -3065,7 +3158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -3154,7 +3247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -3243,7 +3336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -3335,7 +3428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -3424,7 +3517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -3513,7 +3606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -3602,7 +3695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -3691,7 +3784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -3780,7 +3873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -3869,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -3958,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -4047,7 +4140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -4136,7 +4229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>65</v>
       </c>
@@ -4225,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>66</v>
       </c>
@@ -4314,7 +4407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>67</v>
       </c>
@@ -4403,7 +4496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>68</v>
       </c>
@@ -4492,7 +4585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>69</v>
       </c>
@@ -4581,7 +4674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>70</v>
       </c>
@@ -4670,7 +4763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>71</v>
       </c>
@@ -4759,7 +4852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>72</v>
       </c>
@@ -4848,7 +4941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>73</v>
       </c>
@@ -4940,7 +5033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>74</v>
       </c>
@@ -5032,7 +5125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>75</v>
       </c>
@@ -5121,7 +5214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
@@ -5210,7 +5303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:30">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>77</v>
       </c>
@@ -5299,7 +5392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:30">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>78</v>
       </c>
@@ -5388,7 +5481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:30">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>79</v>
       </c>
@@ -5477,7 +5570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:30">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>80</v>
       </c>
@@ -5566,7 +5659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:30">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>81</v>
       </c>
@@ -5655,7 +5748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:30">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>82</v>
       </c>
@@ -5744,7 +5837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:30">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>83</v>
       </c>
@@ -5833,7 +5926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:30">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>84</v>
       </c>
@@ -5922,7 +6015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:30">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>85</v>
       </c>
@@ -6011,7 +6104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>86</v>
       </c>
@@ -6100,7 +6193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:30">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>87</v>
       </c>
@@ -6189,7 +6282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:30">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>88</v>
       </c>
@@ -6278,7 +6371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:30">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>89</v>
       </c>
@@ -6367,7 +6460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:30">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>90</v>
       </c>
@@ -6456,7 +6549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:30">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>91</v>
       </c>
@@ -6545,7 +6638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:30">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>92</v>
       </c>
@@ -6634,7 +6727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:30">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>93</v>
       </c>
@@ -6723,7 +6816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:30">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>94</v>
       </c>
@@ -6812,7 +6905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:30">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>95</v>
       </c>
@@ -6901,7 +6994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:30">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>96</v>
       </c>
@@ -6990,7 +7083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:30">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>97</v>
       </c>
@@ -7079,7 +7172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:30">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>98</v>
       </c>
@@ -7168,7 +7261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:30">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>99</v>
       </c>
@@ -7257,7 +7350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:30">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>100</v>
       </c>
@@ -7346,7 +7439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:30">
+    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>101</v>
       </c>
@@ -7435,7 +7528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:30">
+    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>102</v>
       </c>
@@ -7527,7 +7620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:30">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>103</v>
       </c>
@@ -7619,7 +7712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:30">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>104</v>
       </c>
@@ -7711,7 +7804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:30">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>105</v>
       </c>
@@ -7803,7 +7896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:30">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>106</v>
       </c>
@@ -7892,7 +7985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:30">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>107</v>
       </c>
@@ -7981,7 +8074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:30">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>108</v>
       </c>
@@ -8070,7 +8163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:30">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>109</v>
       </c>
@@ -8159,7 +8252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:30">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>110</v>
       </c>
@@ -8248,7 +8341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:30">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>111</v>
       </c>
@@ -8337,7 +8430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:30">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>112</v>
       </c>
@@ -8426,7 +8519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:30">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>113</v>
       </c>
@@ -8515,7 +8608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:30">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>114</v>
       </c>
@@ -8604,7 +8697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:30">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>115</v>
       </c>
@@ -8693,7 +8786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:30">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>116</v>
       </c>
@@ -8782,7 +8875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:30">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>117</v>
       </c>
@@ -8871,7 +8964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:30">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>118</v>
       </c>
@@ -8960,7 +9053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:30">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>119</v>
       </c>
@@ -9049,7 +9142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>120</v>
       </c>
@@ -9138,7 +9231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:30">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>121</v>
       </c>
@@ -9227,7 +9320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:30">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>122</v>
       </c>
@@ -9316,7 +9409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:30">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>123</v>
       </c>
@@ -9405,7 +9498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:30">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>124</v>
       </c>
@@ -9494,7 +9587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:30">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>125</v>
       </c>
@@ -9583,7 +9676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:30">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>126</v>
       </c>
@@ -9672,7 +9765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:30">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>127</v>
       </c>
@@ -9761,7 +9854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:30">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>128</v>
       </c>
@@ -9850,7 +9943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>129</v>
       </c>
@@ -9939,7 +10032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:30">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>130</v>
       </c>
@@ -10028,7 +10121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>131</v>
       </c>
@@ -10117,7 +10210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>132</v>
       </c>
@@ -10206,7 +10299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:30">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>133</v>
       </c>
@@ -10295,7 +10388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>134</v>
       </c>
@@ -10382,6 +10475,2961 @@
       </c>
       <c r="AD106">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079084CB-492F-B44C-AB65-51FBF4BE0A7A}">
+  <dimension ref="A1:K84"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>1.0961311819999999</v>
+      </c>
+      <c r="C2">
+        <v>1.1113703749999999</v>
+      </c>
+      <c r="D2">
+        <v>1.1113703749999999</v>
+      </c>
+      <c r="E2">
+        <v>1.1075605770000001</v>
+      </c>
+      <c r="F2">
+        <v>1.1151801729999999</v>
+      </c>
+      <c r="G2">
+        <v>1.1075605770000001</v>
+      </c>
+      <c r="H2">
+        <v>1.1113703749999999</v>
+      </c>
+      <c r="I2">
+        <v>1.1113703749999999</v>
+      </c>
+      <c r="J2">
+        <v>-1.517390359</v>
+      </c>
+      <c r="K2">
+        <v>0.48275367800000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>2.6099429770000002</v>
+      </c>
+      <c r="C3">
+        <v>2.650421787</v>
+      </c>
+      <c r="D3">
+        <v>2.650421787</v>
+      </c>
+      <c r="E3">
+        <v>2.646373906</v>
+      </c>
+      <c r="F3">
+        <v>2.646373906</v>
+      </c>
+      <c r="G3">
+        <v>2.646373906</v>
+      </c>
+      <c r="H3">
+        <v>2.650421787</v>
+      </c>
+      <c r="I3">
+        <v>2.650421787</v>
+      </c>
+      <c r="J3">
+        <v>3.9093127550000002</v>
+      </c>
+      <c r="K3">
+        <v>-1.045293501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4">
+        <v>-0.65982804700000008</v>
+      </c>
+      <c r="C4">
+        <v>-0.64874215099999999</v>
+      </c>
+      <c r="D4">
+        <v>-0.65428509899999998</v>
+      </c>
+      <c r="E4">
+        <v>-0.63211330799999998</v>
+      </c>
+      <c r="F4">
+        <v>-0.64042772999999997</v>
+      </c>
+      <c r="G4">
+        <v>-0.65428509899999998</v>
+      </c>
+      <c r="H4">
+        <v>-0.64874215099999999</v>
+      </c>
+      <c r="I4">
+        <v>-0.64874215099999999</v>
+      </c>
+      <c r="J4">
+        <v>-0.61825593899999998</v>
+      </c>
+      <c r="K4">
+        <v>1.2220027149999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>0.195340653</v>
+      </c>
+      <c r="C5">
+        <v>0.215412944</v>
+      </c>
+      <c r="D5">
+        <v>0.215412944</v>
+      </c>
+      <c r="E5">
+        <v>0.205376799</v>
+      </c>
+      <c r="F5">
+        <v>0.215412944</v>
+      </c>
+      <c r="G5">
+        <v>0.215412944</v>
+      </c>
+      <c r="H5">
+        <v>0.215412944</v>
+      </c>
+      <c r="I5">
+        <v>0.215412944</v>
+      </c>
+      <c r="J5">
+        <v>-1.0357598720000001</v>
+      </c>
+      <c r="K5">
+        <v>-0.51722568299999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>-0.49405958100000003</v>
+      </c>
+      <c r="C6">
+        <v>-0.50389918700000003</v>
+      </c>
+      <c r="D6">
+        <v>-0.50061931900000001</v>
+      </c>
+      <c r="E6">
+        <v>-0.51045892500000001</v>
+      </c>
+      <c r="F6">
+        <v>-0.50389918700000003</v>
+      </c>
+      <c r="G6">
+        <v>-0.50389918700000003</v>
+      </c>
+      <c r="H6">
+        <v>-0.50061931900000001</v>
+      </c>
+      <c r="I6">
+        <v>-0.50061931900000001</v>
+      </c>
+      <c r="J6">
+        <v>-1.845365554</v>
+      </c>
+      <c r="K6">
+        <v>-0.40550312100000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7">
+        <v>2.7650806590000001</v>
+      </c>
+      <c r="C7">
+        <v>2.779709215</v>
+      </c>
+      <c r="D7">
+        <v>2.779709215</v>
+      </c>
+      <c r="E7">
+        <v>2.797994911</v>
+      </c>
+      <c r="F7">
+        <v>2.787023494</v>
+      </c>
+      <c r="G7">
+        <v>2.779709215</v>
+      </c>
+      <c r="H7">
+        <v>2.7833663550000001</v>
+      </c>
+      <c r="I7">
+        <v>2.7833663550000001</v>
+      </c>
+      <c r="J7">
+        <v>2.2055383659999999</v>
+      </c>
+      <c r="K7">
+        <v>0.74999697799999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8">
+        <v>0.86265926299999995</v>
+      </c>
+      <c r="C8">
+        <v>0.87018603500000002</v>
+      </c>
+      <c r="D8">
+        <v>0.87018603500000002</v>
+      </c>
+      <c r="E8">
+        <v>0.8664226490000001</v>
+      </c>
+      <c r="F8">
+        <v>0.87018603500000002</v>
+      </c>
+      <c r="G8">
+        <v>0.87018603500000002</v>
+      </c>
+      <c r="H8">
+        <v>0.87018603500000002</v>
+      </c>
+      <c r="I8">
+        <v>0.87018603500000002</v>
+      </c>
+      <c r="J8">
+        <v>1.920170648</v>
+      </c>
+      <c r="K8">
+        <v>2.3491966199999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>1.4075702619999999</v>
+      </c>
+      <c r="C9">
+        <v>1.4075702619999999</v>
+      </c>
+      <c r="D9">
+        <v>1.4103118269999999</v>
+      </c>
+      <c r="E9">
+        <v>1.4075702619999999</v>
+      </c>
+      <c r="F9">
+        <v>1.4130533919999999</v>
+      </c>
+      <c r="G9">
+        <v>1.4075702619999999</v>
+      </c>
+      <c r="H9">
+        <v>1.4103118269999999</v>
+      </c>
+      <c r="I9">
+        <v>1.4130533919999999</v>
+      </c>
+      <c r="J9">
+        <v>3.1950704879999998</v>
+      </c>
+      <c r="K9">
+        <v>-7.0771549999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10">
+        <v>1.1851082310000001</v>
+      </c>
+      <c r="C10">
+        <v>1.192611952</v>
+      </c>
+      <c r="D10">
+        <v>1.188860091</v>
+      </c>
+      <c r="E10">
+        <v>1.1851082310000001</v>
+      </c>
+      <c r="F10">
+        <v>1.2001156740000001</v>
+      </c>
+      <c r="G10">
+        <v>1.188860091</v>
+      </c>
+      <c r="H10">
+        <v>1.188860091</v>
+      </c>
+      <c r="I10">
+        <v>1.192611952</v>
+      </c>
+      <c r="J10">
+        <v>1.046289383</v>
+      </c>
+      <c r="K10">
+        <v>2.1380808610000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>1.100688066</v>
+      </c>
+      <c r="C11">
+        <v>1.100688066</v>
+      </c>
+      <c r="D11">
+        <v>1.100688066</v>
+      </c>
+      <c r="E11">
+        <v>1.100688066</v>
+      </c>
+      <c r="F11">
+        <v>1.0933583529999999</v>
+      </c>
+      <c r="G11">
+        <v>1.0970232099999999</v>
+      </c>
+      <c r="H11">
+        <v>1.0970232099999999</v>
+      </c>
+      <c r="I11">
+        <v>1.0970232099999999</v>
+      </c>
+      <c r="J11">
+        <v>-2.4139093740000002</v>
+      </c>
+      <c r="K11">
+        <v>0.54362986899999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12">
+        <v>0.38458772899999999</v>
+      </c>
+      <c r="C12">
+        <v>0.37139283200000001</v>
+      </c>
+      <c r="D12">
+        <v>0.37139283200000001</v>
+      </c>
+      <c r="E12">
+        <v>0.37799028000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.37469155599999998</v>
+      </c>
+      <c r="G12">
+        <v>0.37799028000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.37469155599999998</v>
+      </c>
+      <c r="I12">
+        <v>0.37469155599999998</v>
+      </c>
+      <c r="J12">
+        <v>-0.24216986900000001</v>
+      </c>
+      <c r="K12">
+        <v>5.1416585000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>0.350535663</v>
+      </c>
+      <c r="C13">
+        <v>0.36740532599999998</v>
+      </c>
+      <c r="D13">
+        <v>0.36740532599999998</v>
+      </c>
+      <c r="E13">
+        <v>0.36065746100000001</v>
+      </c>
+      <c r="F13">
+        <v>0.37077925900000003</v>
+      </c>
+      <c r="G13">
+        <v>0.36740532599999998</v>
+      </c>
+      <c r="H13">
+        <v>0.36065746100000001</v>
+      </c>
+      <c r="I13">
+        <v>0.36065746100000001</v>
+      </c>
+      <c r="J13">
+        <v>-1.650206386</v>
+      </c>
+      <c r="K13">
+        <v>0.40114465199999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14">
+        <v>-0.20491791200000001</v>
+      </c>
+      <c r="C14">
+        <v>-0.162418489</v>
+      </c>
+      <c r="D14">
+        <v>-0.16666843100000001</v>
+      </c>
+      <c r="E14">
+        <v>-0.1836682</v>
+      </c>
+      <c r="F14">
+        <v>-0.16666843100000001</v>
+      </c>
+      <c r="G14">
+        <v>-0.16666843100000001</v>
+      </c>
+      <c r="H14">
+        <v>-0.16666843100000001</v>
+      </c>
+      <c r="I14">
+        <v>-0.16666843100000001</v>
+      </c>
+      <c r="J14">
+        <v>2.4257963880000002</v>
+      </c>
+      <c r="K14">
+        <v>0.47082291799999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15">
+        <v>-0.49640909300000002</v>
+      </c>
+      <c r="C15">
+        <v>-0.49850889799999998</v>
+      </c>
+      <c r="D15">
+        <v>-0.49640909300000002</v>
+      </c>
+      <c r="E15">
+        <v>-0.49220948299999989</v>
+      </c>
+      <c r="F15">
+        <v>-0.48800987400000001</v>
+      </c>
+      <c r="G15">
+        <v>-0.49640909300000002</v>
+      </c>
+      <c r="H15">
+        <v>-0.49640909300000002</v>
+      </c>
+      <c r="I15">
+        <v>-0.49640909300000002</v>
+      </c>
+      <c r="J15">
+        <v>-1.3006343410000001</v>
+      </c>
+      <c r="K15">
+        <v>1.3493193489999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>0.68340353700000001</v>
+      </c>
+      <c r="C16">
+        <v>0.69442408799999999</v>
+      </c>
+      <c r="D16">
+        <v>0.69809760499999995</v>
+      </c>
+      <c r="E16">
+        <v>0.68707705400000008</v>
+      </c>
+      <c r="F16">
+        <v>0.68707705400000008</v>
+      </c>
+      <c r="G16">
+        <v>0.69809760499999995</v>
+      </c>
+      <c r="H16">
+        <v>0.69809760499999995</v>
+      </c>
+      <c r="I16">
+        <v>0.69809760499999995</v>
+      </c>
+      <c r="J16">
+        <v>-2.652150067</v>
+      </c>
+      <c r="K16">
+        <v>-0.984373265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17">
+        <v>-0.265030351</v>
+      </c>
+      <c r="C17">
+        <v>-0.25164229100000002</v>
+      </c>
+      <c r="D17">
+        <v>-0.25164229100000002</v>
+      </c>
+      <c r="E17">
+        <v>-0.25164229100000002</v>
+      </c>
+      <c r="F17">
+        <v>-0.25164229100000002</v>
+      </c>
+      <c r="G17">
+        <v>-0.25164229100000002</v>
+      </c>
+      <c r="H17">
+        <v>-0.25164229100000002</v>
+      </c>
+      <c r="I17">
+        <v>-0.25164229100000002</v>
+      </c>
+      <c r="J17">
+        <v>-1.6138774250000001</v>
+      </c>
+      <c r="K17">
+        <v>-0.64659007000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18">
+        <v>-0.912670278</v>
+      </c>
+      <c r="C18">
+        <v>-0.92797865599999996</v>
+      </c>
+      <c r="D18">
+        <v>-0.92797865599999996</v>
+      </c>
+      <c r="E18">
+        <v>-0.93180574999999999</v>
+      </c>
+      <c r="F18">
+        <v>-0.92797865599999996</v>
+      </c>
+      <c r="G18">
+        <v>-0.92797865599999996</v>
+      </c>
+      <c r="H18">
+        <v>-0.92797865599999996</v>
+      </c>
+      <c r="I18">
+        <v>-0.92797865599999996</v>
+      </c>
+      <c r="J18">
+        <v>-3.0711514709999999</v>
+      </c>
+      <c r="K18">
+        <v>-2.2789429480000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19">
+        <v>-3.3221329000000001E-2</v>
+      </c>
+      <c r="C19">
+        <v>-3.0216423999999999E-2</v>
+      </c>
+      <c r="D19">
+        <v>-2.7211519999999999E-2</v>
+      </c>
+      <c r="E19">
+        <v>-3.0216423999999999E-2</v>
+      </c>
+      <c r="F19">
+        <v>-3.0216423999999999E-2</v>
+      </c>
+      <c r="G19">
+        <v>-3.0216423999999999E-2</v>
+      </c>
+      <c r="H19">
+        <v>-3.0216423999999999E-2</v>
+      </c>
+      <c r="I19">
+        <v>-3.0216423999999999E-2</v>
+      </c>
+      <c r="J19">
+        <v>-2.5513311189999999</v>
+      </c>
+      <c r="K19">
+        <v>-2.1005954770000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20">
+        <v>2.0007049999999998E-2</v>
+      </c>
+      <c r="C20">
+        <v>1.1955318E-2</v>
+      </c>
+      <c r="D20">
+        <v>1.1955318E-2</v>
+      </c>
+      <c r="E20">
+        <v>3.903587E-3</v>
+      </c>
+      <c r="F20">
+        <v>1.1955318E-2</v>
+      </c>
+      <c r="G20">
+        <v>1.1955318E-2</v>
+      </c>
+      <c r="H20">
+        <v>1.1955318E-2</v>
+      </c>
+      <c r="I20">
+        <v>1.1955318E-2</v>
+      </c>
+      <c r="J20">
+        <v>0.22532619500000001</v>
+      </c>
+      <c r="K20">
+        <v>0.32597283500000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21">
+        <v>0.461087521</v>
+      </c>
+      <c r="C21">
+        <v>0.461087521</v>
+      </c>
+      <c r="D21">
+        <v>0.461087521</v>
+      </c>
+      <c r="E21">
+        <v>0.461087521</v>
+      </c>
+      <c r="F21">
+        <v>0.461087521</v>
+      </c>
+      <c r="G21">
+        <v>0.461087521</v>
+      </c>
+      <c r="H21">
+        <v>0.461087521</v>
+      </c>
+      <c r="I21">
+        <v>0.461087521</v>
+      </c>
+      <c r="J21">
+        <v>2.3187317250000001</v>
+      </c>
+      <c r="K21">
+        <v>-0.283625077</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22">
+        <v>0.97356416800000001</v>
+      </c>
+      <c r="C22">
+        <v>0.97747605999999998</v>
+      </c>
+      <c r="D22">
+        <v>0.97747605999999998</v>
+      </c>
+      <c r="E22">
+        <v>0.96965227700000001</v>
+      </c>
+      <c r="F22">
+        <v>0.98529984199999998</v>
+      </c>
+      <c r="G22">
+        <v>0.97747605999999998</v>
+      </c>
+      <c r="H22">
+        <v>0.97747605999999998</v>
+      </c>
+      <c r="I22">
+        <v>0.97747605999999998</v>
+      </c>
+      <c r="J22">
+        <v>-1.811702422</v>
+      </c>
+      <c r="K22">
+        <v>3.2620205659999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>0.83113174599999995</v>
+      </c>
+      <c r="C23">
+        <v>0.85653983099999997</v>
+      </c>
+      <c r="D23">
+        <v>0.85653983099999997</v>
+      </c>
+      <c r="E23">
+        <v>0.83677798700000006</v>
+      </c>
+      <c r="F23">
+        <v>0.86500919300000001</v>
+      </c>
+      <c r="G23">
+        <v>0.85653983099999997</v>
+      </c>
+      <c r="H23">
+        <v>0.85089358999999998</v>
+      </c>
+      <c r="I23">
+        <v>0.85089358999999998</v>
+      </c>
+      <c r="J23">
+        <v>-0.96719607400000007</v>
+      </c>
+      <c r="K23">
+        <v>2.8383704889999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24">
+        <v>1.2791847249999999</v>
+      </c>
+      <c r="C24">
+        <v>1.2751671280000001</v>
+      </c>
+      <c r="D24">
+        <v>1.2751671280000001</v>
+      </c>
+      <c r="E24">
+        <v>1.2791847249999999</v>
+      </c>
+      <c r="F24">
+        <v>1.2791847249999999</v>
+      </c>
+      <c r="G24">
+        <v>1.2791847249999999</v>
+      </c>
+      <c r="H24">
+        <v>1.2791847249999999</v>
+      </c>
+      <c r="I24">
+        <v>1.2791847249999999</v>
+      </c>
+      <c r="J24">
+        <v>3.026839582</v>
+      </c>
+      <c r="K24">
+        <v>0.96179453299999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25">
+        <v>0.76204440699999998</v>
+      </c>
+      <c r="C25">
+        <v>0.76204440699999998</v>
+      </c>
+      <c r="D25">
+        <v>0.76638435099999991</v>
+      </c>
+      <c r="E25">
+        <v>0.75770446299999994</v>
+      </c>
+      <c r="F25">
+        <v>0.76638435099999991</v>
+      </c>
+      <c r="G25">
+        <v>0.76204440699999998</v>
+      </c>
+      <c r="H25">
+        <v>0.76204440699999998</v>
+      </c>
+      <c r="I25">
+        <v>0.76204440699999998</v>
+      </c>
+      <c r="J25">
+        <v>-0.58333818100000001</v>
+      </c>
+      <c r="K25">
+        <v>2.185545984</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>-1.1231730849999999</v>
+      </c>
+      <c r="C26">
+        <v>-1.1231730849999999</v>
+      </c>
+      <c r="D26">
+        <v>-1.1168605119999999</v>
+      </c>
+      <c r="E26">
+        <v>-1.129485657</v>
+      </c>
+      <c r="F26">
+        <v>-1.129485657</v>
+      </c>
+      <c r="G26">
+        <v>-1.120016798</v>
+      </c>
+      <c r="H26">
+        <v>-1.1231730849999999</v>
+      </c>
+      <c r="I26">
+        <v>-1.1231730849999999</v>
+      </c>
+      <c r="J26">
+        <v>2.2445843540000001</v>
+      </c>
+      <c r="K26">
+        <v>-2.575064764</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27">
+        <v>0.81882406200000002</v>
+      </c>
+      <c r="C27">
+        <v>0.81487724900000003</v>
+      </c>
+      <c r="D27">
+        <v>0.81487724900000003</v>
+      </c>
+      <c r="E27">
+        <v>0.79908999599999997</v>
+      </c>
+      <c r="F27">
+        <v>0.81882406200000002</v>
+      </c>
+      <c r="G27">
+        <v>0.81487724900000003</v>
+      </c>
+      <c r="H27">
+        <v>0.81487724900000003</v>
+      </c>
+      <c r="I27">
+        <v>0.81487724900000003</v>
+      </c>
+      <c r="J27">
+        <v>-1.5374234010000001</v>
+      </c>
+      <c r="K27">
+        <v>1.051686039</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28">
+        <v>-0.30726684100000001</v>
+      </c>
+      <c r="C28">
+        <v>-0.30726684100000001</v>
+      </c>
+      <c r="D28">
+        <v>-0.30726684100000001</v>
+      </c>
+      <c r="E28">
+        <v>-0.30726684100000001</v>
+      </c>
+      <c r="F28">
+        <v>-0.30103274499999999</v>
+      </c>
+      <c r="G28">
+        <v>-0.30726684100000001</v>
+      </c>
+      <c r="H28">
+        <v>-0.30726684100000001</v>
+      </c>
+      <c r="I28">
+        <v>-0.30726684100000001</v>
+      </c>
+      <c r="J28">
+        <v>-1.4605745990000001</v>
+      </c>
+      <c r="K28">
+        <v>1.170213908</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29">
+        <v>0.56889458000000004</v>
+      </c>
+      <c r="C29">
+        <v>0.56889458000000004</v>
+      </c>
+      <c r="D29">
+        <v>0.56889458000000004</v>
+      </c>
+      <c r="E29">
+        <v>0.56889458000000004</v>
+      </c>
+      <c r="F29">
+        <v>0.56889458000000004</v>
+      </c>
+      <c r="G29">
+        <v>0.56889458000000004</v>
+      </c>
+      <c r="H29">
+        <v>0.56889458000000004</v>
+      </c>
+      <c r="I29">
+        <v>0.56889458000000004</v>
+      </c>
+      <c r="J29">
+        <v>3.2630243210000001</v>
+      </c>
+      <c r="K29">
+        <v>0.88774770099999989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30">
+        <v>-0.58342863700000003</v>
+      </c>
+      <c r="C30">
+        <v>-0.57254886599999999</v>
+      </c>
+      <c r="D30">
+        <v>-0.56710898100000007</v>
+      </c>
+      <c r="E30">
+        <v>-0.58342863700000003</v>
+      </c>
+      <c r="F30">
+        <v>-0.57254886599999999</v>
+      </c>
+      <c r="G30">
+        <v>-0.57798875199999999</v>
+      </c>
+      <c r="H30">
+        <v>-0.57798875199999999</v>
+      </c>
+      <c r="I30">
+        <v>-0.57798875199999999</v>
+      </c>
+      <c r="J30">
+        <v>0.73030371599999999</v>
+      </c>
+      <c r="K30">
+        <v>1.638764597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31">
+        <v>1.873981833</v>
+      </c>
+      <c r="C31">
+        <v>1.8703830960000001</v>
+      </c>
+      <c r="D31">
+        <v>1.8703830960000001</v>
+      </c>
+      <c r="E31">
+        <v>1.8595868849999999</v>
+      </c>
+      <c r="F31">
+        <v>1.8703830960000001</v>
+      </c>
+      <c r="G31">
+        <v>1.8703830960000001</v>
+      </c>
+      <c r="H31">
+        <v>1.8703830960000001</v>
+      </c>
+      <c r="I31">
+        <v>1.8703830960000001</v>
+      </c>
+      <c r="J31">
+        <v>1.5392992860000001</v>
+      </c>
+      <c r="K31">
+        <v>1.377356118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32">
+        <v>0.19587668699999999</v>
+      </c>
+      <c r="C32">
+        <v>0.19587668699999999</v>
+      </c>
+      <c r="D32">
+        <v>0.19587668699999999</v>
+      </c>
+      <c r="E32">
+        <v>0.218934622</v>
+      </c>
+      <c r="F32">
+        <v>0.19971967600000001</v>
+      </c>
+      <c r="G32">
+        <v>0.19971967600000001</v>
+      </c>
+      <c r="H32">
+        <v>0.19971967600000001</v>
+      </c>
+      <c r="I32">
+        <v>0.19971967600000001</v>
+      </c>
+      <c r="J32">
+        <v>-2.6248773440000002</v>
+      </c>
+      <c r="K32">
+        <v>0.65319239500000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33">
+        <v>-0.51836649800000001</v>
+      </c>
+      <c r="C33">
+        <v>-0.51000199899999998</v>
+      </c>
+      <c r="D33">
+        <v>-0.507213833</v>
+      </c>
+      <c r="E33">
+        <v>-0.51836649800000001</v>
+      </c>
+      <c r="F33">
+        <v>-0.51279016600000005</v>
+      </c>
+      <c r="G33">
+        <v>-0.507213833</v>
+      </c>
+      <c r="H33">
+        <v>-0.51000199899999998</v>
+      </c>
+      <c r="I33">
+        <v>-0.51000199899999998</v>
+      </c>
+      <c r="J33">
+        <v>-2.4394130600000001</v>
+      </c>
+      <c r="K33">
+        <v>-2.174537264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34">
+        <v>1.1748809929999999</v>
+      </c>
+      <c r="C34">
+        <v>1.1832087920000001</v>
+      </c>
+      <c r="D34">
+        <v>1.1832087920000001</v>
+      </c>
+      <c r="E34">
+        <v>1.1748809929999999</v>
+      </c>
+      <c r="F34">
+        <v>1.1790448929999999</v>
+      </c>
+      <c r="G34">
+        <v>1.1832087920000001</v>
+      </c>
+      <c r="H34">
+        <v>1.1832087920000001</v>
+      </c>
+      <c r="I34">
+        <v>1.1832087920000001</v>
+      </c>
+      <c r="J34">
+        <v>4.955701511</v>
+      </c>
+      <c r="K34">
+        <v>0.82511345599999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35">
+        <v>0.57830867600000002</v>
+      </c>
+      <c r="C35">
+        <v>0.58221285200000006</v>
+      </c>
+      <c r="D35">
+        <v>0.57830867600000002</v>
+      </c>
+      <c r="E35">
+        <v>0.59002120400000002</v>
+      </c>
+      <c r="F35">
+        <v>0.58611702799999998</v>
+      </c>
+      <c r="G35">
+        <v>0.57830867600000002</v>
+      </c>
+      <c r="H35">
+        <v>0.58221285200000006</v>
+      </c>
+      <c r="I35">
+        <v>0.58221285200000006</v>
+      </c>
+      <c r="J35">
+        <v>-1.6275508000000001</v>
+      </c>
+      <c r="K35">
+        <v>-1.69782597</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36">
+        <v>-0.75982305599999989</v>
+      </c>
+      <c r="C36">
+        <v>-0.75982305599999989</v>
+      </c>
+      <c r="D36">
+        <v>-0.74911368900000008</v>
+      </c>
+      <c r="E36">
+        <v>-0.73572698200000008</v>
+      </c>
+      <c r="F36">
+        <v>-0.74911368900000008</v>
+      </c>
+      <c r="G36">
+        <v>-0.74375900599999989</v>
+      </c>
+      <c r="H36">
+        <v>-0.75446837300000003</v>
+      </c>
+      <c r="I36">
+        <v>-0.75446837300000003</v>
+      </c>
+      <c r="J36">
+        <v>-0.70092154099999993</v>
+      </c>
+      <c r="K36">
+        <v>0.72610152599999989</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>1.1205018330000001</v>
+      </c>
+      <c r="C37">
+        <v>1.137617791</v>
+      </c>
+      <c r="D37">
+        <v>1.137617791</v>
+      </c>
+      <c r="E37">
+        <v>1.137617791</v>
+      </c>
+      <c r="F37">
+        <v>1.1205018330000001</v>
+      </c>
+      <c r="G37">
+        <v>1.1273482159999999</v>
+      </c>
+      <c r="H37">
+        <v>1.137617791</v>
+      </c>
+      <c r="I37">
+        <v>1.137617791</v>
+      </c>
+      <c r="J37">
+        <v>0.58990713500000003</v>
+      </c>
+      <c r="K37">
+        <v>2.2570014459999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38">
+        <v>0.45298592500000001</v>
+      </c>
+      <c r="C38">
+        <v>0.47259013100000002</v>
+      </c>
+      <c r="D38">
+        <v>0.47259013100000002</v>
+      </c>
+      <c r="E38">
+        <v>0.45858712699999998</v>
+      </c>
+      <c r="F38">
+        <v>0.47259013100000002</v>
+      </c>
+      <c r="G38">
+        <v>0.47259013100000002</v>
+      </c>
+      <c r="H38">
+        <v>0.47259013100000002</v>
+      </c>
+      <c r="I38">
+        <v>0.47259013100000002</v>
+      </c>
+      <c r="J38">
+        <v>-0.74287065400000007</v>
+      </c>
+      <c r="K38">
+        <v>1.8112773559999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39">
+        <v>1.501966964</v>
+      </c>
+      <c r="C39">
+        <v>1.510348384</v>
+      </c>
+      <c r="D39">
+        <v>1.501966964</v>
+      </c>
+      <c r="E39">
+        <v>1.501966964</v>
+      </c>
+      <c r="F39">
+        <v>1.501966964</v>
+      </c>
+      <c r="G39">
+        <v>1.510348384</v>
+      </c>
+      <c r="H39">
+        <v>1.506157674</v>
+      </c>
+      <c r="I39">
+        <v>1.506157674</v>
+      </c>
+      <c r="J39">
+        <v>2.1515270160000002</v>
+      </c>
+      <c r="K39">
+        <v>1.552255484</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>0.53859577800000003</v>
+      </c>
+      <c r="C40">
+        <v>0.54221051799999997</v>
+      </c>
+      <c r="D40">
+        <v>0.54221051799999997</v>
+      </c>
+      <c r="E40">
+        <v>0.53498103799999996</v>
+      </c>
+      <c r="F40">
+        <v>0.54221051799999997</v>
+      </c>
+      <c r="G40">
+        <v>0.54221051799999997</v>
+      </c>
+      <c r="H40">
+        <v>0.54221051799999997</v>
+      </c>
+      <c r="I40">
+        <v>0.54221051799999997</v>
+      </c>
+      <c r="J40">
+        <v>-0.1482049</v>
+      </c>
+      <c r="K40">
+        <v>0.26749024700000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41">
+        <v>2.4551379309999999</v>
+      </c>
+      <c r="C41">
+        <v>2.4801366570000001</v>
+      </c>
+      <c r="D41">
+        <v>2.4801366570000001</v>
+      </c>
+      <c r="E41">
+        <v>2.4619557649999999</v>
+      </c>
+      <c r="F41">
+        <v>2.4778640460000001</v>
+      </c>
+      <c r="G41">
+        <v>2.471046211</v>
+      </c>
+      <c r="H41">
+        <v>2.4801366570000001</v>
+      </c>
+      <c r="I41">
+        <v>2.4801366570000001</v>
+      </c>
+      <c r="J41">
+        <v>3.9596067439999998</v>
+      </c>
+      <c r="K41">
+        <v>-1.858278696</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42">
+        <v>-0.20563748400000001</v>
+      </c>
+      <c r="C42">
+        <v>-0.20563748400000001</v>
+      </c>
+      <c r="D42">
+        <v>-0.20563748400000001</v>
+      </c>
+      <c r="E42">
+        <v>-0.21500619400000001</v>
+      </c>
+      <c r="F42">
+        <v>-0.20563748400000001</v>
+      </c>
+      <c r="G42">
+        <v>-0.21032183900000001</v>
+      </c>
+      <c r="H42">
+        <v>-0.20563748400000001</v>
+      </c>
+      <c r="I42">
+        <v>-0.20563748400000001</v>
+      </c>
+      <c r="J42">
+        <v>-1.151877145</v>
+      </c>
+      <c r="K42">
+        <v>0.27216670100000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43">
+        <v>-1.5142783339999999</v>
+      </c>
+      <c r="C43">
+        <v>-1.5282854290000001</v>
+      </c>
+      <c r="D43">
+        <v>-1.5282854290000001</v>
+      </c>
+      <c r="E43">
+        <v>-1.5310868479999999</v>
+      </c>
+      <c r="F43">
+        <v>-1.5142783339999999</v>
+      </c>
+      <c r="G43">
+        <v>-1.52548401</v>
+      </c>
+      <c r="H43">
+        <v>-1.52548401</v>
+      </c>
+      <c r="I43">
+        <v>-1.52548401</v>
+      </c>
+      <c r="J43">
+        <v>-3.147505566</v>
+      </c>
+      <c r="K43">
+        <v>-1.738391848</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44">
+        <v>-0.7871949840000001</v>
+      </c>
+      <c r="C44">
+        <v>-0.75594056099999996</v>
+      </c>
+      <c r="D44">
+        <v>-0.75594056099999996</v>
+      </c>
+      <c r="E44">
+        <v>-0.77469321499999999</v>
+      </c>
+      <c r="F44">
+        <v>-0.77156777200000004</v>
+      </c>
+      <c r="G44">
+        <v>-0.77156777200000004</v>
+      </c>
+      <c r="H44">
+        <v>-0.77156777200000004</v>
+      </c>
+      <c r="I44">
+        <v>-0.77156777200000004</v>
+      </c>
+      <c r="J44">
+        <v>2.3632509270000002</v>
+      </c>
+      <c r="K44">
+        <v>2.5420031999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45">
+        <v>0.75718812599999996</v>
+      </c>
+      <c r="C45">
+        <v>0.78087066099999991</v>
+      </c>
+      <c r="D45">
+        <v>0.77410422200000006</v>
+      </c>
+      <c r="E45">
+        <v>0.76395456400000006</v>
+      </c>
+      <c r="F45">
+        <v>0.77072100300000002</v>
+      </c>
+      <c r="G45">
+        <v>0.77748744099999989</v>
+      </c>
+      <c r="H45">
+        <v>0.77748744099999989</v>
+      </c>
+      <c r="I45">
+        <v>0.77748744099999989</v>
+      </c>
+      <c r="J45">
+        <v>-2.494085562</v>
+      </c>
+      <c r="K45">
+        <v>1.9277819819999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46">
+        <v>0.55977697000000004</v>
+      </c>
+      <c r="C46">
+        <v>0.56340687499999997</v>
+      </c>
+      <c r="D46">
+        <v>0.55977697000000004</v>
+      </c>
+      <c r="E46">
+        <v>0.54162744699999998</v>
+      </c>
+      <c r="F46">
+        <v>0.55977697000000004</v>
+      </c>
+      <c r="G46">
+        <v>0.55977697000000004</v>
+      </c>
+      <c r="H46">
+        <v>0.55977697000000004</v>
+      </c>
+      <c r="I46">
+        <v>0.55977697000000004</v>
+      </c>
+      <c r="J46">
+        <v>-1.6980236959999999</v>
+      </c>
+      <c r="K46">
+        <v>1.754015586</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47">
+        <v>-0.42818149</v>
+      </c>
+      <c r="C47">
+        <v>-0.40637804500000002</v>
+      </c>
+      <c r="D47">
+        <v>-0.40637804500000002</v>
+      </c>
+      <c r="E47">
+        <v>-0.40637804500000002</v>
+      </c>
+      <c r="F47">
+        <v>-0.40637804500000002</v>
+      </c>
+      <c r="G47">
+        <v>-0.40637804500000002</v>
+      </c>
+      <c r="H47">
+        <v>-0.40637804500000002</v>
+      </c>
+      <c r="I47">
+        <v>-0.40637804500000002</v>
+      </c>
+      <c r="J47">
+        <v>2.2584873650000001</v>
+      </c>
+      <c r="K47">
+        <v>0.97208415299999995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48">
+        <v>-1.001239843</v>
+      </c>
+      <c r="C48">
+        <v>-1.004619822</v>
+      </c>
+      <c r="D48">
+        <v>-1.004619822</v>
+      </c>
+      <c r="E48">
+        <v>-0.99785986400000004</v>
+      </c>
+      <c r="F48">
+        <v>-1.001239843</v>
+      </c>
+      <c r="G48">
+        <v>-1.001239843</v>
+      </c>
+      <c r="H48">
+        <v>-1.001239843</v>
+      </c>
+      <c r="I48">
+        <v>-1.001239843</v>
+      </c>
+      <c r="J48">
+        <v>-1.379797505</v>
+      </c>
+      <c r="K48">
+        <v>0.56369049399999993</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49">
+        <v>-1.947792427</v>
+      </c>
+      <c r="C49">
+        <v>-1.9527176589999999</v>
+      </c>
+      <c r="D49">
+        <v>-1.955180275</v>
+      </c>
+      <c r="E49">
+        <v>-1.947792427</v>
+      </c>
+      <c r="F49">
+        <v>-1.95764289</v>
+      </c>
+      <c r="G49">
+        <v>-1.955180275</v>
+      </c>
+      <c r="H49">
+        <v>-1.955180275</v>
+      </c>
+      <c r="I49">
+        <v>-1.955180275</v>
+      </c>
+      <c r="J49">
+        <v>-1.0046105940000001</v>
+      </c>
+      <c r="K49">
+        <v>-2.5511332869999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50">
+        <v>1.04895925</v>
+      </c>
+      <c r="C50">
+        <v>1.0522569399999999</v>
+      </c>
+      <c r="D50">
+        <v>1.0522569399999999</v>
+      </c>
+      <c r="E50">
+        <v>1.058852321</v>
+      </c>
+      <c r="F50">
+        <v>1.0522569399999999</v>
+      </c>
+      <c r="G50">
+        <v>1.0522569399999999</v>
+      </c>
+      <c r="H50">
+        <v>1.0522569399999999</v>
+      </c>
+      <c r="I50">
+        <v>1.0522569399999999</v>
+      </c>
+      <c r="J50">
+        <v>0.67961796799999996</v>
+      </c>
+      <c r="K50">
+        <v>3.436486828</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51">
+        <v>0.58371325399999996</v>
+      </c>
+      <c r="C51">
+        <v>0.58062313300000001</v>
+      </c>
+      <c r="D51">
+        <v>0.58062313300000001</v>
+      </c>
+      <c r="E51">
+        <v>0.58680337500000002</v>
+      </c>
+      <c r="F51">
+        <v>0.58680337500000002</v>
+      </c>
+      <c r="G51">
+        <v>0.58680337500000002</v>
+      </c>
+      <c r="H51">
+        <v>0.58680337500000002</v>
+      </c>
+      <c r="I51">
+        <v>0.58680337500000002</v>
+      </c>
+      <c r="J51">
+        <v>5.2212450000000001E-2</v>
+      </c>
+      <c r="K51">
+        <v>1.501479177</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52">
+        <v>6.3778527000000002E-2</v>
+      </c>
+      <c r="C52">
+        <v>9.3336368000000003E-2</v>
+      </c>
+      <c r="D52">
+        <v>8.4469015999999994E-2</v>
+      </c>
+      <c r="E52">
+        <v>6.6734310999999991E-2</v>
+      </c>
+      <c r="F52">
+        <v>8.4469015999999994E-2</v>
+      </c>
+      <c r="G52">
+        <v>9.3336368000000003E-2</v>
+      </c>
+      <c r="H52">
+        <v>8.4469015999999994E-2</v>
+      </c>
+      <c r="I52">
+        <v>8.4469015999999994E-2</v>
+      </c>
+      <c r="J52">
+        <v>-0.23771146000000001</v>
+      </c>
+      <c r="K52">
+        <v>1.3052078810000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53">
+        <v>-1.10167521</v>
+      </c>
+      <c r="C53">
+        <v>-1.1087825769999999</v>
+      </c>
+      <c r="D53">
+        <v>-1.1087825769999999</v>
+      </c>
+      <c r="E53">
+        <v>-1.0969369659999999</v>
+      </c>
+      <c r="F53">
+        <v>-1.1111517</v>
+      </c>
+      <c r="G53">
+        <v>-1.106413455</v>
+      </c>
+      <c r="H53">
+        <v>-1.1087825769999999</v>
+      </c>
+      <c r="I53">
+        <v>-1.1087825769999999</v>
+      </c>
+      <c r="J53">
+        <v>-1.324372713</v>
+      </c>
+      <c r="K53">
+        <v>1.075548247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54">
+        <v>1.05322494</v>
+      </c>
+      <c r="C54">
+        <v>1.0559481529999999</v>
+      </c>
+      <c r="D54">
+        <v>1.0559481529999999</v>
+      </c>
+      <c r="E54">
+        <v>1.0586713670000001</v>
+      </c>
+      <c r="F54">
+        <v>1.0586713670000001</v>
+      </c>
+      <c r="G54">
+        <v>1.0559481529999999</v>
+      </c>
+      <c r="H54">
+        <v>1.0586713670000001</v>
+      </c>
+      <c r="I54">
+        <v>1.0586713670000001</v>
+      </c>
+      <c r="J54">
+        <v>-0.33289088999999999</v>
+      </c>
+      <c r="K54">
+        <v>-1.250613945</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55">
+        <v>0.26485910699999998</v>
+      </c>
+      <c r="C55">
+        <v>0.27571130700000002</v>
+      </c>
+      <c r="D55">
+        <v>0.27571130700000002</v>
+      </c>
+      <c r="E55">
+        <v>0.27842435700000001</v>
+      </c>
+      <c r="F55">
+        <v>0.27842435700000001</v>
+      </c>
+      <c r="G55">
+        <v>0.27299825700000002</v>
+      </c>
+      <c r="H55">
+        <v>0.27571130700000002</v>
+      </c>
+      <c r="I55">
+        <v>0.27571130700000002</v>
+      </c>
+      <c r="J55">
+        <v>-1.019793E-3</v>
+      </c>
+      <c r="K55">
+        <v>0.131919657</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56">
+        <v>0.23854713</v>
+      </c>
+      <c r="C56">
+        <v>0.24981815399999999</v>
+      </c>
+      <c r="D56">
+        <v>0.24418264200000001</v>
+      </c>
+      <c r="E56">
+        <v>0.24981815399999999</v>
+      </c>
+      <c r="F56">
+        <v>0.24981815399999999</v>
+      </c>
+      <c r="G56">
+        <v>0.24981815399999999</v>
+      </c>
+      <c r="H56">
+        <v>0.24418264200000001</v>
+      </c>
+      <c r="I56">
+        <v>0.24418264200000001</v>
+      </c>
+      <c r="J56">
+        <v>-1.860681139</v>
+      </c>
+      <c r="K56">
+        <v>-0.22920037700000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57">
+        <v>-7.8201822000000004E-2</v>
+      </c>
+      <c r="C57">
+        <v>-6.8058137000000005E-2</v>
+      </c>
+      <c r="D57">
+        <v>-7.1439365000000005E-2</v>
+      </c>
+      <c r="E57">
+        <v>-5.7914450999999999E-2</v>
+      </c>
+      <c r="F57">
+        <v>-6.4676907999999991E-2</v>
+      </c>
+      <c r="G57">
+        <v>-6.8058137000000005E-2</v>
+      </c>
+      <c r="H57">
+        <v>-7.1439365000000005E-2</v>
+      </c>
+      <c r="I57">
+        <v>-7.1439365000000005E-2</v>
+      </c>
+      <c r="J57">
+        <v>0.351214199</v>
+      </c>
+      <c r="K57">
+        <v>-0.28783798999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58">
+        <v>1.101260533</v>
+      </c>
+      <c r="C58">
+        <v>1.101260533</v>
+      </c>
+      <c r="D58">
+        <v>1.0977666850000001</v>
+      </c>
+      <c r="E58">
+        <v>1.0907789910000001</v>
+      </c>
+      <c r="F58">
+        <v>1.108248227</v>
+      </c>
+      <c r="G58">
+        <v>1.101260533</v>
+      </c>
+      <c r="H58">
+        <v>1.101260533</v>
+      </c>
+      <c r="I58">
+        <v>1.101260533</v>
+      </c>
+      <c r="J58">
+        <v>-3.444234673</v>
+      </c>
+      <c r="K58">
+        <v>2.1039946789999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59">
+        <v>0.32366270800000002</v>
+      </c>
+      <c r="C59">
+        <v>0.32697264100000001</v>
+      </c>
+      <c r="D59">
+        <v>0.32697264100000001</v>
+      </c>
+      <c r="E59">
+        <v>0.33028257500000002</v>
+      </c>
+      <c r="F59">
+        <v>0.32697264100000001</v>
+      </c>
+      <c r="G59">
+        <v>0.32697264100000001</v>
+      </c>
+      <c r="H59">
+        <v>0.32697264100000001</v>
+      </c>
+      <c r="I59">
+        <v>0.32697264100000001</v>
+      </c>
+      <c r="J59">
+        <v>1.932290343</v>
+      </c>
+      <c r="K59">
+        <v>-1.9105423399999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B60">
+        <v>0.79397555500000006</v>
+      </c>
+      <c r="C60">
+        <v>0.81818150700000003</v>
+      </c>
+      <c r="D60">
+        <v>0.81472351300000001</v>
+      </c>
+      <c r="E60">
+        <v>0.80089154099999993</v>
+      </c>
+      <c r="F60">
+        <v>0.81818150700000003</v>
+      </c>
+      <c r="G60">
+        <v>0.81126551999999996</v>
+      </c>
+      <c r="H60">
+        <v>0.81126551999999996</v>
+      </c>
+      <c r="I60">
+        <v>0.81126551999999996</v>
+      </c>
+      <c r="J60">
+        <v>1.3818343719999999</v>
+      </c>
+      <c r="K60">
+        <v>1.565108003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61">
+        <v>-1.0865290700000001</v>
+      </c>
+      <c r="C61">
+        <v>-1.095492377</v>
+      </c>
+      <c r="D61">
+        <v>-1.095492377</v>
+      </c>
+      <c r="E61">
+        <v>-1.095492377</v>
+      </c>
+      <c r="F61">
+        <v>-1.095492377</v>
+      </c>
+      <c r="G61">
+        <v>-1.09325155</v>
+      </c>
+      <c r="H61">
+        <v>-1.09325155</v>
+      </c>
+      <c r="I61">
+        <v>-1.09325155</v>
+      </c>
+      <c r="J61">
+        <v>9.6627355999999998E-2</v>
+      </c>
+      <c r="K61">
+        <v>-1.149272214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62">
+        <v>2.1801233</v>
+      </c>
+      <c r="C62">
+        <v>2.1801233</v>
+      </c>
+      <c r="D62">
+        <v>2.1801233</v>
+      </c>
+      <c r="E62">
+        <v>2.1801233</v>
+      </c>
+      <c r="F62">
+        <v>2.1801233</v>
+      </c>
+      <c r="G62">
+        <v>2.1801233</v>
+      </c>
+      <c r="H62">
+        <v>2.1801233</v>
+      </c>
+      <c r="I62">
+        <v>2.1801233</v>
+      </c>
+      <c r="J62">
+        <v>1.9117107019999999</v>
+      </c>
+      <c r="K62">
+        <v>0.89621637400000009</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63">
+        <v>1.3952471799999999</v>
+      </c>
+      <c r="C63">
+        <v>1.408922131</v>
+      </c>
+      <c r="D63">
+        <v>1.412340868</v>
+      </c>
+      <c r="E63">
+        <v>1.408922131</v>
+      </c>
+      <c r="F63">
+        <v>1.408922131</v>
+      </c>
+      <c r="G63">
+        <v>1.412340868</v>
+      </c>
+      <c r="H63">
+        <v>1.412340868</v>
+      </c>
+      <c r="I63">
+        <v>1.412340868</v>
+      </c>
+      <c r="J63">
+        <v>1.00892983</v>
+      </c>
+      <c r="K63">
+        <v>1.8020769560000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64">
+        <v>0.67390470099999999</v>
+      </c>
+      <c r="C64">
+        <v>0.68871755999999995</v>
+      </c>
+      <c r="D64">
+        <v>0.68871755999999995</v>
+      </c>
+      <c r="E64">
+        <v>0.67760791599999992</v>
+      </c>
+      <c r="F64">
+        <v>0.68871755999999995</v>
+      </c>
+      <c r="G64">
+        <v>0.68871755999999995</v>
+      </c>
+      <c r="H64">
+        <v>0.68871755999999995</v>
+      </c>
+      <c r="I64">
+        <v>0.68871755999999995</v>
+      </c>
+      <c r="J64">
+        <v>-2.7330529270000001</v>
+      </c>
+      <c r="K64">
+        <v>-2.1331321270000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65">
+        <v>0.107490904</v>
+      </c>
+      <c r="C65">
+        <v>0.10416449</v>
+      </c>
+      <c r="D65">
+        <v>0.107490904</v>
+      </c>
+      <c r="E65">
+        <v>9.7511660999999999E-2</v>
+      </c>
+      <c r="F65">
+        <v>0.10416449</v>
+      </c>
+      <c r="G65">
+        <v>0.10416449</v>
+      </c>
+      <c r="H65">
+        <v>0.10416449</v>
+      </c>
+      <c r="I65">
+        <v>0.10416449</v>
+      </c>
+      <c r="J65">
+        <v>-0.88045414599999994</v>
+      </c>
+      <c r="K65">
+        <v>-1.5124728650000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66">
+        <v>-0.48155015400000001</v>
+      </c>
+      <c r="C66">
+        <v>-0.47788983499999999</v>
+      </c>
+      <c r="D66">
+        <v>-0.48155015400000001</v>
+      </c>
+      <c r="E66">
+        <v>-0.47056919700000011</v>
+      </c>
+      <c r="F66">
+        <v>-0.48155015400000001</v>
+      </c>
+      <c r="G66">
+        <v>-0.48521047299999998</v>
+      </c>
+      <c r="H66">
+        <v>-0.48155015400000001</v>
+      </c>
+      <c r="I66">
+        <v>-0.48155015400000001</v>
+      </c>
+      <c r="J66">
+        <v>-2.8021923050000002</v>
+      </c>
+      <c r="K66">
+        <v>-0.99765511200000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B67">
+        <v>1.2225072960000001</v>
+      </c>
+      <c r="C67">
+        <v>1.218973595</v>
+      </c>
+      <c r="D67">
+        <v>1.2225072960000001</v>
+      </c>
+      <c r="E67">
+        <v>1.204838793</v>
+      </c>
+      <c r="F67">
+        <v>1.2225072960000001</v>
+      </c>
+      <c r="G67">
+        <v>1.218973595</v>
+      </c>
+      <c r="H67">
+        <v>1.2225072960000001</v>
+      </c>
+      <c r="I67">
+        <v>1.2225072960000001</v>
+      </c>
+      <c r="J67">
+        <v>-0.47366894500000001</v>
+      </c>
+      <c r="K67">
+        <v>1.7419612689999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68">
+        <v>-1.52334349</v>
+      </c>
+      <c r="C68">
+        <v>-1.512646224</v>
+      </c>
+      <c r="D68">
+        <v>-1.509971908</v>
+      </c>
+      <c r="E68">
+        <v>-1.5179948569999999</v>
+      </c>
+      <c r="F68">
+        <v>-1.509971908</v>
+      </c>
+      <c r="G68">
+        <v>-1.512646224</v>
+      </c>
+      <c r="H68">
+        <v>-1.5153205409999999</v>
+      </c>
+      <c r="I68">
+        <v>-1.5153205409999999</v>
+      </c>
+      <c r="J68">
+        <v>-2.1945969010000002</v>
+      </c>
+      <c r="K68">
+        <v>0.134732665</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69">
+        <v>2.7072501529999999</v>
+      </c>
+      <c r="C69">
+        <v>2.7338319200000001</v>
+      </c>
+      <c r="D69">
+        <v>2.737629316</v>
+      </c>
+      <c r="E69">
+        <v>2.7338319200000001</v>
+      </c>
+      <c r="F69">
+        <v>2.752818897</v>
+      </c>
+      <c r="G69">
+        <v>2.737629316</v>
+      </c>
+      <c r="H69">
+        <v>2.737629316</v>
+      </c>
+      <c r="I69">
+        <v>2.737629316</v>
+      </c>
+      <c r="J69">
+        <v>4.0895020750000004</v>
+      </c>
+      <c r="K69">
+        <v>-1.1205244029999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70">
+        <v>0.140181795</v>
+      </c>
+      <c r="C70">
+        <v>0.12605375699999999</v>
+      </c>
+      <c r="D70">
+        <v>0.13311777599999999</v>
+      </c>
+      <c r="E70">
+        <v>0.11192571799999999</v>
+      </c>
+      <c r="F70">
+        <v>0.12605375699999999</v>
+      </c>
+      <c r="G70">
+        <v>0.12605375699999999</v>
+      </c>
+      <c r="H70">
+        <v>0.115457728</v>
+      </c>
+      <c r="I70">
+        <v>0.115457728</v>
+      </c>
+      <c r="J70">
+        <v>-0.72516055999999995</v>
+      </c>
+      <c r="K70">
+        <v>-2.3604810120000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71">
+        <v>0.31131919400000002</v>
+      </c>
+      <c r="C71">
+        <v>0.29617712000000002</v>
+      </c>
+      <c r="D71">
+        <v>0.29617712000000002</v>
+      </c>
+      <c r="E71">
+        <v>0.29617712000000002</v>
+      </c>
+      <c r="F71">
+        <v>0.29617712000000002</v>
+      </c>
+      <c r="G71">
+        <v>0.29617712000000002</v>
+      </c>
+      <c r="H71">
+        <v>0.29617712000000002</v>
+      </c>
+      <c r="I71">
+        <v>0.29617712000000002</v>
+      </c>
+      <c r="J71">
+        <v>-3.2546393060000001</v>
+      </c>
+      <c r="K71">
+        <v>2.3517137080000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72">
+        <v>-0.69231576500000003</v>
+      </c>
+      <c r="C72">
+        <v>-0.65946866400000004</v>
+      </c>
+      <c r="D72">
+        <v>-0.66416110700000008</v>
+      </c>
+      <c r="E72">
+        <v>-0.657122443</v>
+      </c>
+      <c r="F72">
+        <v>-0.66181488600000005</v>
+      </c>
+      <c r="G72">
+        <v>-0.66181488600000005</v>
+      </c>
+      <c r="H72">
+        <v>-0.66416110700000008</v>
+      </c>
+      <c r="I72">
+        <v>-0.66416110700000008</v>
+      </c>
+      <c r="J72">
+        <v>0.23444172699999999</v>
+      </c>
+      <c r="K72">
+        <v>0.9805401640000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73">
+        <v>1.4666651639999999</v>
+      </c>
+      <c r="C73">
+        <v>1.4822834579999999</v>
+      </c>
+      <c r="D73">
+        <v>1.474474311</v>
+      </c>
+      <c r="E73">
+        <v>1.458856017</v>
+      </c>
+      <c r="F73">
+        <v>1.474474311</v>
+      </c>
+      <c r="G73">
+        <v>1.474474311</v>
+      </c>
+      <c r="H73">
+        <v>1.474474311</v>
+      </c>
+      <c r="I73">
+        <v>1.474474311</v>
+      </c>
+      <c r="J73">
+        <v>-0.35286606999999998</v>
+      </c>
+      <c r="K73">
+        <v>2.81374301</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B74">
+        <v>-0.511421193</v>
+      </c>
+      <c r="C74">
+        <v>-0.52606668099999998</v>
+      </c>
+      <c r="D74">
+        <v>-0.52606668099999998</v>
+      </c>
+      <c r="E74">
+        <v>-0.53338942499999997</v>
+      </c>
+      <c r="F74">
+        <v>-0.52972805299999992</v>
+      </c>
+      <c r="G74">
+        <v>-0.52972805299999992</v>
+      </c>
+      <c r="H74">
+        <v>-0.52972805299999992</v>
+      </c>
+      <c r="I74">
+        <v>-0.52972805299999992</v>
+      </c>
+      <c r="J74">
+        <v>-4.9526655239999986</v>
+      </c>
+      <c r="K74">
+        <v>-0.52606668099999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75">
+        <v>-0.96390392599999997</v>
+      </c>
+      <c r="C75">
+        <v>-0.93820953200000001</v>
+      </c>
+      <c r="D75">
+        <v>-0.94391939800000002</v>
+      </c>
+      <c r="E75">
+        <v>-0.93535460000000004</v>
+      </c>
+      <c r="F75">
+        <v>-0.93535460000000004</v>
+      </c>
+      <c r="G75">
+        <v>-0.93820953200000001</v>
+      </c>
+      <c r="H75">
+        <v>-0.94391939800000002</v>
+      </c>
+      <c r="I75">
+        <v>-0.94391939800000002</v>
+      </c>
+      <c r="J75">
+        <v>-1.252252127</v>
+      </c>
+      <c r="K75">
+        <v>1.3257520819999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76">
+        <v>-0.48777247400000001</v>
+      </c>
+      <c r="C76">
+        <v>-0.48777247400000001</v>
+      </c>
+      <c r="D76">
+        <v>-0.48777247400000001</v>
+      </c>
+      <c r="E76">
+        <v>-0.48777247400000001</v>
+      </c>
+      <c r="F76">
+        <v>-0.50385322200000004</v>
+      </c>
+      <c r="G76">
+        <v>-0.48777247400000001</v>
+      </c>
+      <c r="H76">
+        <v>-0.48777247400000001</v>
+      </c>
+      <c r="I76">
+        <v>-0.48777247400000001</v>
+      </c>
+      <c r="J76">
+        <v>-1.6262894370000001</v>
+      </c>
+      <c r="K76">
+        <v>0.73114822900000009</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77">
+        <v>-0.10667998200000001</v>
+      </c>
+      <c r="C77">
+        <v>-0.10667998200000001</v>
+      </c>
+      <c r="D77">
+        <v>-0.10667998200000001</v>
+      </c>
+      <c r="E77">
+        <v>-0.10667998200000001</v>
+      </c>
+      <c r="F77">
+        <v>-0.10667998200000001</v>
+      </c>
+      <c r="G77">
+        <v>-0.10667998200000001</v>
+      </c>
+      <c r="H77">
+        <v>-0.10667998200000001</v>
+      </c>
+      <c r="I77">
+        <v>-0.10667998200000001</v>
+      </c>
+      <c r="J77">
+        <v>2.5188598999999999E-2</v>
+      </c>
+      <c r="K77">
+        <v>-1.177327273</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B78">
+        <v>-6.5838424000000006E-2</v>
+      </c>
+      <c r="C78">
+        <v>-5.5892667E-2</v>
+      </c>
+      <c r="D78">
+        <v>-6.5838424000000006E-2</v>
+      </c>
+      <c r="E78">
+        <v>-5.5892667E-2</v>
+      </c>
+      <c r="F78">
+        <v>-6.2523172000000002E-2</v>
+      </c>
+      <c r="G78">
+        <v>-5.5892667E-2</v>
+      </c>
+      <c r="H78">
+        <v>-6.2523172000000002E-2</v>
+      </c>
+      <c r="I78">
+        <v>-6.2523172000000002E-2</v>
+      </c>
+      <c r="J78">
+        <v>-2.1875997819999999</v>
+      </c>
+      <c r="K78">
+        <v>0.70993057299999995</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B79">
+        <v>0.65584967900000002</v>
+      </c>
+      <c r="C79">
+        <v>0.65814258999999997</v>
+      </c>
+      <c r="D79">
+        <v>0.65584967900000002</v>
+      </c>
+      <c r="E79">
+        <v>0.65584967900000002</v>
+      </c>
+      <c r="F79">
+        <v>0.651263857</v>
+      </c>
+      <c r="G79">
+        <v>0.65814258999999997</v>
+      </c>
+      <c r="H79">
+        <v>0.65584967900000002</v>
+      </c>
+      <c r="I79">
+        <v>0.65584967900000002</v>
+      </c>
+      <c r="J79">
+        <v>-1.969533682</v>
+      </c>
+      <c r="K79">
+        <v>1.307036469</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B80">
+        <v>-0.55221196500000003</v>
+      </c>
+      <c r="C80">
+        <v>-0.54774936500000004</v>
+      </c>
+      <c r="D80">
+        <v>-0.55221196500000003</v>
+      </c>
+      <c r="E80">
+        <v>-0.55221196500000003</v>
+      </c>
+      <c r="F80">
+        <v>-0.55667456500000001</v>
+      </c>
+      <c r="G80">
+        <v>-0.54774936500000004</v>
+      </c>
+      <c r="H80">
+        <v>-0.55221196500000003</v>
+      </c>
+      <c r="I80">
+        <v>-0.55221196500000003</v>
+      </c>
+      <c r="J80">
+        <v>0.67946561500000002</v>
+      </c>
+      <c r="K80">
+        <v>0.48757381799999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B81">
+        <v>-0.39855983499999997</v>
+      </c>
+      <c r="C81">
+        <v>-0.39260141399999998</v>
+      </c>
+      <c r="D81">
+        <v>-0.39260141399999998</v>
+      </c>
+      <c r="E81">
+        <v>-0.39260141399999998</v>
+      </c>
+      <c r="F81">
+        <v>-0.39558062500000002</v>
+      </c>
+      <c r="G81">
+        <v>-0.39260141399999998</v>
+      </c>
+      <c r="H81">
+        <v>-0.39260141399999998</v>
+      </c>
+      <c r="I81">
+        <v>-0.39260141399999998</v>
+      </c>
+      <c r="J81">
+        <v>-2.5048616579999998</v>
+      </c>
+      <c r="K81">
+        <v>0.69481041799999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B82">
+        <v>0.59858450899999993</v>
+      </c>
+      <c r="C82">
+        <v>0.60669745799999997</v>
+      </c>
+      <c r="D82">
+        <v>0.60399314199999998</v>
+      </c>
+      <c r="E82">
+        <v>0.60399314199999998</v>
+      </c>
+      <c r="F82">
+        <v>0.60399314199999998</v>
+      </c>
+      <c r="G82">
+        <v>0.60669745799999997</v>
+      </c>
+      <c r="H82">
+        <v>0.60399314199999998</v>
+      </c>
+      <c r="I82">
+        <v>0.60399314199999998</v>
+      </c>
+      <c r="J82">
+        <v>-0.60213190999999999</v>
+      </c>
+      <c r="K82">
+        <v>2.7782634129999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83">
+        <v>-0.19128452700000001</v>
+      </c>
+      <c r="C83">
+        <v>-0.18391768</v>
+      </c>
+      <c r="D83">
+        <v>-0.18602249400000001</v>
+      </c>
+      <c r="E83">
+        <v>-0.18602249400000001</v>
+      </c>
+      <c r="F83">
+        <v>-0.167079173</v>
+      </c>
+      <c r="G83">
+        <v>-0.18391768</v>
+      </c>
+      <c r="H83">
+        <v>-0.18602249400000001</v>
+      </c>
+      <c r="I83">
+        <v>-0.18602249400000001</v>
+      </c>
+      <c r="J83">
+        <v>-0.34072628199999999</v>
+      </c>
+      <c r="K83">
+        <v>1.3673298309999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B84">
+        <v>0.56697529400000002</v>
+      </c>
+      <c r="C84">
+        <v>0.57870170499999996</v>
+      </c>
+      <c r="D84">
+        <v>0.57674730299999999</v>
+      </c>
+      <c r="E84">
+        <v>0.57674730299999999</v>
+      </c>
+      <c r="F84">
+        <v>0.57674730299999999</v>
+      </c>
+      <c r="G84">
+        <v>0.57870170499999996</v>
+      </c>
+      <c r="H84">
+        <v>0.57674730299999999</v>
+      </c>
+      <c r="I84">
+        <v>0.57674730299999999</v>
+      </c>
+      <c r="J84">
+        <v>-0.205013429</v>
+      </c>
+      <c r="K84">
+        <v>3.2151897730000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>